<commit_message>
7/10 class work seet 3
</commit_message>
<xml_diff>
--- a/excel_data.xlsx
+++ b/excel_data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abhi Bhalodia\Desktop\excle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B32A51-FC73-438C-86E0-13B401098BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A71D850C-24EE-4866-9449-E2FFA0C38935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{5AE2433E-C0DB-4218-B298-848E7350EA34}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{5AE2433E-C0DB-4218-B298-848E7350EA34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="83">
   <si>
     <t>Name</t>
   </si>
@@ -202,6 +203,87 @@
   </si>
   <si>
     <t>E</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Abhi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> komal</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Shivani</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Taksh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ixit</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>BIO</t>
+  </si>
+  <si>
+    <t>MATHS</t>
+  </si>
+  <si>
+    <t>PHYSICS</t>
+  </si>
+  <si>
+    <t>MORE THEN 80 IN MATHS</t>
+  </si>
+  <si>
+    <t>MORE THEN 80 IN BIO</t>
+  </si>
+  <si>
+    <t>MORE THEN 80 BIO &amp; MAT.</t>
+  </si>
+  <si>
+    <t>AVE. MARKES OF MATHS</t>
+  </si>
+  <si>
+    <t>AVE. MARKES OF BIO</t>
+  </si>
+  <si>
+    <t>AVE. MARKES OF PHYSICS</t>
+  </si>
+  <si>
+    <t>MORETHEN AVE. IN MATHS</t>
+  </si>
+  <si>
+    <t>MORE THEN AVE. IN BIO</t>
+  </si>
+  <si>
+    <t>MORE THEN AVE. IN PHYSICS</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>PER. OF STUDENT</t>
+  </si>
+  <si>
+    <t>MAX</t>
+  </si>
+  <si>
+    <t>HIGEST MARKES IN MATHS</t>
+  </si>
+  <si>
+    <t>HIGEST MARKES IN BIO</t>
+  </si>
+  <si>
+    <t>HIGEST MARKES IN PHYSICS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAX </t>
+  </si>
+  <si>
+    <t>PASS OR FAIL</t>
+  </si>
+  <si>
+    <t>GREAD</t>
   </si>
 </sst>
 </file>
@@ -294,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -317,6 +399,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3906,8 +3989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18888350-3B9C-4808-ABB0-DEA8DC06A1BA}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4373,4 +4456,488 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E486363-D196-47EC-B0E1-D25DB7D76661}">
+  <dimension ref="A1:K15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="10" max="10" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2">
+        <v>85</v>
+      </c>
+      <c r="C2">
+        <v>56</v>
+      </c>
+      <c r="D2">
+        <v>75</v>
+      </c>
+      <c r="E2">
+        <f>SUM(B2:D2)</f>
+        <v>216</v>
+      </c>
+      <c r="F2" s="10">
+        <f>E2/3</f>
+        <v>72</v>
+      </c>
+      <c r="G2">
+        <f>MAX(B2:D2)</f>
+        <v>85</v>
+      </c>
+      <c r="H2" t="str">
+        <f>IF(OR(B2&lt;35,C2&lt;35,D2&lt;35),"FAIL","PASS")</f>
+        <v>PASS</v>
+      </c>
+      <c r="I2" t="str">
+        <f>IF(H2="FAIL","FAIL",IF(F2&gt;=90,"A",IF(F2&gt;=60,"B",IF(F2&gt;=50,"C"))))</f>
+        <v>B</v>
+      </c>
+      <c r="J2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" s="10">
+        <f>COUNTIF(C2:C10,"&gt;80")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3">
+        <v>96</v>
+      </c>
+      <c r="C3">
+        <v>85</v>
+      </c>
+      <c r="D3">
+        <v>89</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E10" si="0">SUM(B3:D3)</f>
+        <v>270</v>
+      </c>
+      <c r="F3" s="10">
+        <f t="shared" ref="F3:F10" si="1">E3/3</f>
+        <v>90</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G10" si="2">MAX(B3:D3)</f>
+        <v>96</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H10" si="3">IF(OR(B3&lt;35,C3&lt;35,D3&lt;35),"FAIL","PASS")</f>
+        <v>PASS</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I10" si="4">IF(H3="FAIL","FAIL",IF(F3&gt;=90,"A",IF(F3&gt;=60,"B",IF(F3&gt;=50,"C"))))</f>
+        <v>A</v>
+      </c>
+      <c r="J3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K3" s="10">
+        <f>COUNTIF(B2:B10,"&gt;80")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4">
+        <v>78</v>
+      </c>
+      <c r="C4">
+        <v>75</v>
+      </c>
+      <c r="D4">
+        <v>85</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>238</v>
+      </c>
+      <c r="F4" s="10">
+        <f t="shared" si="1"/>
+        <v>79.333333333333329</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>85</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="3"/>
+        <v>PASS</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="4"/>
+        <v>B</v>
+      </c>
+      <c r="J4" t="s">
+        <v>67</v>
+      </c>
+      <c r="K4" s="10">
+        <f>COUNTIFS(C2:C10,"&gt;80",B2:B10,"&gt;80")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5">
+        <v>56</v>
+      </c>
+      <c r="C5">
+        <v>34</v>
+      </c>
+      <c r="D5">
+        <v>68</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>158</v>
+      </c>
+      <c r="F5" s="10">
+        <f t="shared" si="1"/>
+        <v>52.666666666666664</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>68</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="3"/>
+        <v>FAIL</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="4"/>
+        <v>FAIL</v>
+      </c>
+      <c r="J5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K5" s="10">
+        <f>AVERAGE(C2:C10)</f>
+        <v>74.777777777777771</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6">
+        <v>54</v>
+      </c>
+      <c r="C6">
+        <v>85</v>
+      </c>
+      <c r="D6">
+        <v>78</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>217</v>
+      </c>
+      <c r="F6" s="10">
+        <f t="shared" si="1"/>
+        <v>72.333333333333329</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>85</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="3"/>
+        <v>PASS</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="4"/>
+        <v>B</v>
+      </c>
+      <c r="J6" t="s">
+        <v>70</v>
+      </c>
+      <c r="K6" s="10">
+        <f>AVERAGE(D2:D10)</f>
+        <v>77.888888888888886</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <v>78</v>
+      </c>
+      <c r="D7">
+        <v>78</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>186</v>
+      </c>
+      <c r="F7" s="10">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>78</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="3"/>
+        <v>FAIL</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="4"/>
+        <v>FAIL</v>
+      </c>
+      <c r="J7" t="s">
+        <v>69</v>
+      </c>
+      <c r="K7" s="10">
+        <f>AVERAGE(B2:B10)</f>
+        <v>64.333333333333329</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8">
+        <v>52</v>
+      </c>
+      <c r="C8">
+        <v>98</v>
+      </c>
+      <c r="D8">
+        <v>65</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>215</v>
+      </c>
+      <c r="F8" s="10">
+        <f t="shared" si="1"/>
+        <v>71.666666666666671</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>98</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="3"/>
+        <v>PASS</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="4"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9">
+        <v>63</v>
+      </c>
+      <c r="C9">
+        <v>87</v>
+      </c>
+      <c r="D9">
+        <v>85</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>235</v>
+      </c>
+      <c r="F9" s="10">
+        <f t="shared" si="1"/>
+        <v>78.333333333333329</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>87</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="3"/>
+        <v>PASS</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="4"/>
+        <v>B</v>
+      </c>
+      <c r="J9" t="s">
+        <v>71</v>
+      </c>
+      <c r="K9" s="10">
+        <f>COUNTIF(C2:C10,"&gt;"&amp;K5)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10">
+        <v>65</v>
+      </c>
+      <c r="C10">
+        <v>75</v>
+      </c>
+      <c r="D10">
+        <v>78</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>218</v>
+      </c>
+      <c r="F10" s="10">
+        <f t="shared" si="1"/>
+        <v>72.666666666666671</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>78</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="3"/>
+        <v>PASS</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="4"/>
+        <v>B</v>
+      </c>
+      <c r="J10" t="s">
+        <v>72</v>
+      </c>
+      <c r="K10" s="10">
+        <f>COUNTIF(B2:B10,"&gt;"&amp;K7)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" t="s">
+        <v>76</v>
+      </c>
+      <c r="J11" t="s">
+        <v>73</v>
+      </c>
+      <c r="K11" s="10">
+        <f>COUNTIF(D2:D10,"&gt;"&amp;K6)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <f>MAX(B2:B10)</f>
+        <v>96</v>
+      </c>
+      <c r="C12">
+        <f>MAX(C2:C10)</f>
+        <v>98</v>
+      </c>
+      <c r="D12">
+        <f>MAX(D2:D10)</f>
+        <v>89</v>
+      </c>
+      <c r="F12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F13" s="10">
+        <f>MAX(F2:F10)</f>
+        <v>90</v>
+      </c>
+      <c r="J13" t="s">
+        <v>77</v>
+      </c>
+      <c r="K13" s="10" t="str">
+        <f>LOOKUP(C12,C2:C10,A2:A10)</f>
+        <v>Meera</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" t="str">
+        <f>LOOKUP(B12,B2:B10,A2:A10)</f>
+        <v>Raj</v>
+      </c>
+      <c r="J14" t="s">
+        <v>78</v>
+      </c>
+      <c r="K14" s="10" t="str">
+        <f>LOOKUP(96,B2:B10,A2:A10)</f>
+        <v>Raj</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>79</v>
+      </c>
+      <c r="K15" s="10" t="str">
+        <f>LOOKUP(D12,D1:D10,A1:A10)</f>
+        <v>Raj</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>